<commit_message>
server: add more feeds
</commit_message>
<xml_diff>
--- a/server/cmd/tools/createfeeds/feeds.xlsx
+++ b/server/cmd/tools/createfeeds/feeds.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7215" uniqueCount="3938">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7275" uniqueCount="3968">
   <si>
     <t>TopicCode</t>
   </si>
@@ -11844,6 +11844,96 @@
   </si>
   <si>
     <t>https://rsshub.app/paulgraham/articles</t>
+  </si>
+  <si>
+    <t>The Guardian - Architecture</t>
+  </si>
+  <si>
+    <t>https://www.theguardian.com/artanddesign/architecture/rss</t>
+  </si>
+  <si>
+    <t>https://www.theguardian.com/artanddesign/architecture/</t>
+  </si>
+  <si>
+    <t>WWE - Youtube</t>
+  </si>
+  <si>
+    <t>http://www.youtube.com/feeds/videos.xml?channel_id=UCJ5v_MCY6GNUBTO8-D3XoAg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UCJ5v_MCY6GNUBTO8-D3XoAg</t>
+  </si>
+  <si>
+    <t>r/web</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/web.rss</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/web/</t>
+  </si>
+  <si>
+    <t>r/nosleep</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/nosleep.rss</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/nosleep/</t>
+  </si>
+  <si>
+    <t>The Verge</t>
+  </si>
+  <si>
+    <t>https://www.theverge.com/rss/index.xml</t>
+  </si>
+  <si>
+    <t>https://www.theverge.com/</t>
+  </si>
+  <si>
+    <t>Kent C. Dodds Blog</t>
+  </si>
+  <si>
+    <t>https://kentcdodds.com/blog/rss.xml</t>
+  </si>
+  <si>
+    <t>https://kentcdodds.com/blog</t>
+  </si>
+  <si>
+    <t>Gizmodo</t>
+  </si>
+  <si>
+    <t>https://gizmodo.com/feed</t>
+  </si>
+  <si>
+    <t>https://gizmodo.com/</t>
+  </si>
+  <si>
+    <t>TechCrunch</t>
+  </si>
+  <si>
+    <t>https://techcrunch.com/feed/</t>
+  </si>
+  <si>
+    <t>https://techcrunch.com/</t>
+  </si>
+  <si>
+    <t>decoist</t>
+  </si>
+  <si>
+    <t>https://www.decoist.com/feed/</t>
+  </si>
+  <si>
+    <t>https://www.decoist.com/</t>
+  </si>
+  <si>
+    <t>Zaha Hadid</t>
+  </si>
+  <si>
+    <t>https://www.zaha-hadid.com/feed/</t>
+  </si>
+  <si>
+    <t>https://www.zaha-hadid.com/</t>
   </si>
 </sst>
 </file>
@@ -12233,10 +12323,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1094"/>
+  <dimension ref="A1:F1104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A263" sqref="A263"/>
+    <sheetView tabSelected="1" topLeftCell="A1089" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A1105" sqref="A1105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -34126,6 +34216,206 @@
         <v>598</v>
       </c>
       <c r="F1094" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:6">
+      <c r="A1095" t="s">
+        <v>3938</v>
+      </c>
+      <c r="B1095" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1095" t="s">
+        <v>3939</v>
+      </c>
+      <c r="D1095" s="5" t="s">
+        <v>3940</v>
+      </c>
+      <c r="E1095" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1095" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:6">
+      <c r="A1096" t="s">
+        <v>3941</v>
+      </c>
+      <c r="B1096" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1096" t="s">
+        <v>3942</v>
+      </c>
+      <c r="D1096" t="s">
+        <v>3943</v>
+      </c>
+      <c r="E1096" t="s">
+        <v>564</v>
+      </c>
+      <c r="F1096" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:6">
+      <c r="A1097" t="s">
+        <v>3944</v>
+      </c>
+      <c r="B1097" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C1097" t="s">
+        <v>3945</v>
+      </c>
+      <c r="D1097" s="5" t="s">
+        <v>3946</v>
+      </c>
+      <c r="E1097" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1097" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:6">
+      <c r="A1098" t="s">
+        <v>3947</v>
+      </c>
+      <c r="B1098" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1098" s="5" t="s">
+        <v>3948</v>
+      </c>
+      <c r="D1098" s="5" t="s">
+        <v>3949</v>
+      </c>
+      <c r="E1098" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1098" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:6">
+      <c r="A1099" t="s">
+        <v>3950</v>
+      </c>
+      <c r="B1099" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1099" t="s">
+        <v>3951</v>
+      </c>
+      <c r="D1099" t="s">
+        <v>3952</v>
+      </c>
+      <c r="E1099" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1099" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:6">
+      <c r="A1100" t="s">
+        <v>3953</v>
+      </c>
+      <c r="B1100" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C1100" t="s">
+        <v>3954</v>
+      </c>
+      <c r="D1100" t="s">
+        <v>3955</v>
+      </c>
+      <c r="E1100" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1100" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:6">
+      <c r="A1101" t="s">
+        <v>3956</v>
+      </c>
+      <c r="B1101" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1101" t="s">
+        <v>3957</v>
+      </c>
+      <c r="D1101" s="5" t="s">
+        <v>3958</v>
+      </c>
+      <c r="E1101" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1101" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:6">
+      <c r="A1102" t="s">
+        <v>3959</v>
+      </c>
+      <c r="B1102" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1102" t="s">
+        <v>3960</v>
+      </c>
+      <c r="D1102" s="5" t="s">
+        <v>3961</v>
+      </c>
+      <c r="E1102" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1102" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:6">
+      <c r="A1103" t="s">
+        <v>3962</v>
+      </c>
+      <c r="B1103" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1103" t="s">
+        <v>3963</v>
+      </c>
+      <c r="D1103" s="5" t="s">
+        <v>3964</v>
+      </c>
+      <c r="E1103" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1103" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:6">
+      <c r="A1104" t="s">
+        <v>3965</v>
+      </c>
+      <c r="B1104" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1104" t="s">
+        <v>3966</v>
+      </c>
+      <c r="D1104" s="5" t="s">
+        <v>3967</v>
+      </c>
+      <c r="E1104" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1104" t="s">
         <v>3928</v>
       </c>
     </row>
@@ -34420,9 +34710,17 @@
     <hyperlink ref="D878" r:id="rId269"/>
     <hyperlink ref="D389" r:id="rId270"/>
     <hyperlink ref="D793" r:id="rId271"/>
+    <hyperlink ref="D1095" r:id="rId272"/>
+    <hyperlink ref="D1097" r:id="rId273"/>
+    <hyperlink ref="C1098" r:id="rId274"/>
+    <hyperlink ref="D1098" r:id="rId275"/>
+    <hyperlink ref="D1101" r:id="rId276"/>
+    <hyperlink ref="D1102" r:id="rId277"/>
+    <hyperlink ref="D1103" r:id="rId278"/>
+    <hyperlink ref="D1104" r:id="rId279"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId272"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId280"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>

<commit_message>
server: add architectural subreddit feeds
</commit_message>
<xml_diff>
--- a/server/cmd/tools/createfeeds/feeds.xlsx
+++ b/server/cmd/tools/createfeeds/feeds.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7275" uniqueCount="3968">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7377" uniqueCount="4019">
   <si>
     <t>TopicCode</t>
   </si>
@@ -11934,6 +11934,159 @@
   </si>
   <si>
     <t>https://www.zaha-hadid.com/</t>
+  </si>
+  <si>
+    <t>Tanmay Bhat - Youtube</t>
+  </si>
+  <si>
+    <t>http://www.youtube.com/feeds/videos.xml?channel_id=UC0rE2qq81of4fojo-KhO5rg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UC0rE2qq81of4fojo-KhO5rg</t>
+  </si>
+  <si>
+    <t>r/urbanism</t>
+  </si>
+  <si>
+    <t>r/architectureporn</t>
+  </si>
+  <si>
+    <t>r/architects</t>
+  </si>
+  <si>
+    <t>r/exteriordesign</t>
+  </si>
+  <si>
+    <t>r/cityporn</t>
+  </si>
+  <si>
+    <t>r/urbanhell</t>
+  </si>
+  <si>
+    <t>r/skyscrapers</t>
+  </si>
+  <si>
+    <t>r/centuryhomes</t>
+  </si>
+  <si>
+    <t>r/architecturalrevival</t>
+  </si>
+  <si>
+    <t>r/interiordesign</t>
+  </si>
+  <si>
+    <t>r/architectureportfolio</t>
+  </si>
+  <si>
+    <t>r/amazing_architecture</t>
+  </si>
+  <si>
+    <t>r/brutalism</t>
+  </si>
+  <si>
+    <t>r/artdeco</t>
+  </si>
+  <si>
+    <t>r/floorplan</t>
+  </si>
+  <si>
+    <t>r/urbandesign</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/urbanism/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/architectureporn/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/architects/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/exteriordesign/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/cityporn/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/urbanhell/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/skyscrapers/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/centuryhomes/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/architecturalrevival/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/interiordesign/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/architectureportfolio/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/amazing_architecture/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/brutalism/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/artdeco/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/floorplan/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/urbandesign/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/urbanism.rss</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/architectureporn.rss</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/architects.rss</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/exteriordesign.rss</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/cityporn.rss</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/urbanhell.rss</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/skyscrapers.rss</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/centuryhomes.rss</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/architecturalrevival.rss</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/interiordesign.rss</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/architectureportfolio.rss</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/amazing_architecture.rss</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/brutalism.rss</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/artdeco.rss</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/floorplan.rss</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/urbandesign.rss</t>
   </si>
 </sst>
 </file>
@@ -12323,10 +12476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1104"/>
+  <dimension ref="A1:F1121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1089" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A1105" sqref="A1105"/>
+    <sheetView tabSelected="1" topLeftCell="A1099" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A1107" sqref="A1107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -34416,6 +34569,346 @@
         <v>598</v>
       </c>
       <c r="F1104" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:6">
+      <c r="A1105" t="s">
+        <v>3968</v>
+      </c>
+      <c r="B1105" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1105" t="s">
+        <v>3969</v>
+      </c>
+      <c r="D1105" t="s">
+        <v>3970</v>
+      </c>
+      <c r="E1105" t="s">
+        <v>564</v>
+      </c>
+      <c r="F1105" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:6">
+      <c r="A1106" t="s">
+        <v>3971</v>
+      </c>
+      <c r="B1106" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1106" t="s">
+        <v>4003</v>
+      </c>
+      <c r="D1106" t="s">
+        <v>3987</v>
+      </c>
+      <c r="E1106" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1106" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:6">
+      <c r="A1107" t="s">
+        <v>3972</v>
+      </c>
+      <c r="B1107" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1107" t="s">
+        <v>4004</v>
+      </c>
+      <c r="D1107" t="s">
+        <v>3988</v>
+      </c>
+      <c r="E1107" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1107" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:6">
+      <c r="A1108" t="s">
+        <v>3973</v>
+      </c>
+      <c r="B1108" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1108" t="s">
+        <v>4005</v>
+      </c>
+      <c r="D1108" t="s">
+        <v>3989</v>
+      </c>
+      <c r="E1108" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1108" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:6">
+      <c r="A1109" t="s">
+        <v>3974</v>
+      </c>
+      <c r="B1109" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1109" t="s">
+        <v>4006</v>
+      </c>
+      <c r="D1109" t="s">
+        <v>3990</v>
+      </c>
+      <c r="E1109" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1109" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:6">
+      <c r="A1110" t="s">
+        <v>3975</v>
+      </c>
+      <c r="B1110" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1110" t="s">
+        <v>4007</v>
+      </c>
+      <c r="D1110" t="s">
+        <v>3991</v>
+      </c>
+      <c r="E1110" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1110" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:6">
+      <c r="A1111" t="s">
+        <v>3976</v>
+      </c>
+      <c r="B1111" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1111" t="s">
+        <v>4008</v>
+      </c>
+      <c r="D1111" t="s">
+        <v>3992</v>
+      </c>
+      <c r="E1111" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1111" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:6">
+      <c r="A1112" t="s">
+        <v>3977</v>
+      </c>
+      <c r="B1112" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1112" t="s">
+        <v>4009</v>
+      </c>
+      <c r="D1112" t="s">
+        <v>3993</v>
+      </c>
+      <c r="E1112" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1112" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:6">
+      <c r="A1113" t="s">
+        <v>3978</v>
+      </c>
+      <c r="B1113" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1113" t="s">
+        <v>4010</v>
+      </c>
+      <c r="D1113" t="s">
+        <v>3994</v>
+      </c>
+      <c r="E1113" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1113" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:6">
+      <c r="A1114" t="s">
+        <v>3979</v>
+      </c>
+      <c r="B1114" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1114" t="s">
+        <v>4011</v>
+      </c>
+      <c r="D1114" t="s">
+        <v>3995</v>
+      </c>
+      <c r="E1114" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1114" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:6">
+      <c r="A1115" t="s">
+        <v>3980</v>
+      </c>
+      <c r="B1115" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1115" t="s">
+        <v>4012</v>
+      </c>
+      <c r="D1115" t="s">
+        <v>3996</v>
+      </c>
+      <c r="E1115" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1115" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:6">
+      <c r="A1116" t="s">
+        <v>3981</v>
+      </c>
+      <c r="B1116" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1116" t="s">
+        <v>4013</v>
+      </c>
+      <c r="D1116" t="s">
+        <v>3997</v>
+      </c>
+      <c r="E1116" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1116" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:6">
+      <c r="A1117" t="s">
+        <v>3982</v>
+      </c>
+      <c r="B1117" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1117" t="s">
+        <v>4014</v>
+      </c>
+      <c r="D1117" t="s">
+        <v>3998</v>
+      </c>
+      <c r="E1117" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1117" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:6">
+      <c r="A1118" t="s">
+        <v>3983</v>
+      </c>
+      <c r="B1118" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1118" t="s">
+        <v>4015</v>
+      </c>
+      <c r="D1118" t="s">
+        <v>3999</v>
+      </c>
+      <c r="E1118" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1118" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:6">
+      <c r="A1119" t="s">
+        <v>3984</v>
+      </c>
+      <c r="B1119" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1119" t="s">
+        <v>4016</v>
+      </c>
+      <c r="D1119" t="s">
+        <v>4000</v>
+      </c>
+      <c r="E1119" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1119" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:6">
+      <c r="A1120" t="s">
+        <v>3985</v>
+      </c>
+      <c r="B1120" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1120" t="s">
+        <v>4017</v>
+      </c>
+      <c r="D1120" t="s">
+        <v>4001</v>
+      </c>
+      <c r="E1120" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1120" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:6">
+      <c r="A1121" t="s">
+        <v>3986</v>
+      </c>
+      <c r="B1121" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1121" t="s">
+        <v>4018</v>
+      </c>
+      <c r="D1121" t="s">
+        <v>4002</v>
+      </c>
+      <c r="E1121" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1121" t="s">
         <v>3928</v>
       </c>
     </row>

</xml_diff>

<commit_message>
server: remove arch from design topic and add more feeds
</commit_message>
<xml_diff>
--- a/server/cmd/tools/createfeeds/feeds.xlsx
+++ b/server/cmd/tools/createfeeds/feeds.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7377" uniqueCount="4019">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7467" uniqueCount="4064">
   <si>
     <t>TopicCode</t>
   </si>
@@ -11861,9 +11861,6 @@
     <t>http://www.youtube.com/feeds/videos.xml?channel_id=UCJ5v_MCY6GNUBTO8-D3XoAg</t>
   </si>
   <si>
-    <t>https://www.youtube.com/channel/UCJ5v_MCY6GNUBTO8-D3XoAg</t>
-  </si>
-  <si>
     <t>r/web</t>
   </si>
   <si>
@@ -11942,9 +11939,6 @@
     <t>http://www.youtube.com/feeds/videos.xml?channel_id=UC0rE2qq81of4fojo-KhO5rg</t>
   </si>
   <si>
-    <t>https://www.youtube.com/channel/UC0rE2qq81of4fojo-KhO5rg</t>
-  </si>
-  <si>
     <t>r/urbanism</t>
   </si>
   <si>
@@ -12087,6 +12081,147 @@
   </si>
   <si>
     <t>https://www.reddit.com/r/urbandesign.rss</t>
+  </si>
+  <si>
+    <t>Scratching the Surface - Substack</t>
+  </si>
+  <si>
+    <t>https://surfacepodcast.substack.com/</t>
+  </si>
+  <si>
+    <t>https://surfacepodcast.substack.com/feed</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/cricketshitpost.rss</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/cricketshitpost/</t>
+  </si>
+  <si>
+    <t>r/CricketShitpost</t>
+  </si>
+  <si>
+    <t>https://preppykitchen.com/feed/</t>
+  </si>
+  <si>
+    <t>https://preppykitchen.com/</t>
+  </si>
+  <si>
+    <t>Preppy Kitchen</t>
+  </si>
+  <si>
+    <t>Joy of Baking - Youtube</t>
+  </si>
+  <si>
+    <t>http://www.youtube.com/feeds/videos.xml?channel_id=UCFjd060Z3nTHv0UyO8M43mQ</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@joyofbaking</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@tanmaybhat</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@WWE</t>
+  </si>
+  <si>
+    <t>r/soccer</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/soccer/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/soccer.rss</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@StrayKidsJapanOfficial</t>
+  </si>
+  <si>
+    <t>http://www.youtube.com/feeds/videos.xml?channel_id=UC9rMiEjNaCSsebs31MRDCRA</t>
+  </si>
+  <si>
+    <t>Stray Kids Japan - Youtube</t>
+  </si>
+  <si>
+    <t>https://www.fia.com/rss/press-release</t>
+  </si>
+  <si>
+    <t>https://www.fia.com/news</t>
+  </si>
+  <si>
+    <t>FIA - Press release</t>
+  </si>
+  <si>
+    <t>https://racingnews365.com/feed/news.xml</t>
+  </si>
+  <si>
+    <t>https://racingnews365.com</t>
+  </si>
+  <si>
+    <t>RacingNews365</t>
+  </si>
+  <si>
+    <t>GSMArena</t>
+  </si>
+  <si>
+    <t>https://www.gsmarena.com/rss-news-reviews.php3</t>
+  </si>
+  <si>
+    <t>https://www.gsmarena.com/</t>
+  </si>
+  <si>
+    <t>Upstairs - Youtube</t>
+  </si>
+  <si>
+    <t>http://www.youtube.com/feeds/videos.xml?channel_id=UC1ptLbehYDNqwdnIGwLpysw</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@LearnUpstairs</t>
+  </si>
+  <si>
+    <t>Show it better - Youtube</t>
+  </si>
+  <si>
+    <t>http://www.youtube.com/feeds/videos.xml?channel_id=UC_eRv_Rzr671BaKFtpYSi4A</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@ShowItBetter</t>
+  </si>
+  <si>
+    <t>Fireship</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/@Fireship</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/feeds/videos.xml?channel_id=UCsBjURrPoezykLs9EqgamOA</t>
+  </si>
+  <si>
+    <t>Formula 1</t>
+  </si>
+  <si>
+    <t>https://rss-bridge.org/bridge01/?action=display&amp;bridge=Formula1Bridge&amp;limit=10&amp;format=Atom</t>
+  </si>
+  <si>
+    <t>https://www.formula1.com/</t>
+  </si>
+  <si>
+    <t>arsTECHNICA</t>
+  </si>
+  <si>
+    <t>https://feeds.arstechnica.com/arstechnica/index</t>
+  </si>
+  <si>
+    <t>https://arstechnica.com/</t>
+  </si>
+  <si>
+    <t>KoozArch Magazine</t>
+  </si>
+  <si>
+    <t>https://rss.diffbot.com/rss?url=https://www.koozarch.com/magazine</t>
+  </si>
+  <si>
+    <t>https://www.koozarch.com/magazine</t>
   </si>
 </sst>
 </file>
@@ -12476,10 +12611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1121"/>
+  <dimension ref="A1:F1136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1099" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A1107" sqref="A1107"/>
+    <sheetView tabSelected="1" topLeftCell="A1120" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A1137" sqref="A1137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -13739,7 +13874,7 @@
       <c r="B63" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="5" t="s">
         <v>784</v>
       </c>
       <c r="D63" t="s">
@@ -34403,7 +34538,7 @@
         <v>3942</v>
       </c>
       <c r="D1096" t="s">
-        <v>3943</v>
+        <v>4030</v>
       </c>
       <c r="E1096" t="s">
         <v>564</v>
@@ -34414,16 +34549,16 @@
     </row>
     <row r="1097" spans="1:6">
       <c r="A1097" t="s">
-        <v>3944</v>
+        <v>3943</v>
       </c>
       <c r="B1097" s="3" t="s">
         <v>227</v>
       </c>
       <c r="C1097" t="s">
+        <v>3944</v>
+      </c>
+      <c r="D1097" s="5" t="s">
         <v>3945</v>
-      </c>
-      <c r="D1097" s="5" t="s">
-        <v>3946</v>
       </c>
       <c r="E1097" t="s">
         <v>734</v>
@@ -34434,16 +34569,16 @@
     </row>
     <row r="1098" spans="1:6">
       <c r="A1098" t="s">
-        <v>3947</v>
+        <v>3946</v>
       </c>
       <c r="B1098" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C1098" s="5" t="s">
+        <v>3947</v>
+      </c>
+      <c r="D1098" s="5" t="s">
         <v>3948</v>
-      </c>
-      <c r="D1098" s="5" t="s">
-        <v>3949</v>
       </c>
       <c r="E1098" t="s">
         <v>734</v>
@@ -34454,16 +34589,16 @@
     </row>
     <row r="1099" spans="1:6">
       <c r="A1099" t="s">
-        <v>3950</v>
+        <v>3949</v>
       </c>
       <c r="B1099" s="3" t="s">
         <v>84</v>
       </c>
       <c r="C1099" t="s">
+        <v>3950</v>
+      </c>
+      <c r="D1099" t="s">
         <v>3951</v>
-      </c>
-      <c r="D1099" t="s">
-        <v>3952</v>
       </c>
       <c r="E1099" t="s">
         <v>598</v>
@@ -34474,16 +34609,16 @@
     </row>
     <row r="1100" spans="1:6">
       <c r="A1100" t="s">
-        <v>3953</v>
+        <v>3952</v>
       </c>
       <c r="B1100" s="3" t="s">
         <v>266</v>
       </c>
       <c r="C1100" t="s">
+        <v>3953</v>
+      </c>
+      <c r="D1100" t="s">
         <v>3954</v>
-      </c>
-      <c r="D1100" t="s">
-        <v>3955</v>
       </c>
       <c r="E1100" t="s">
         <v>598</v>
@@ -34494,16 +34629,16 @@
     </row>
     <row r="1101" spans="1:6">
       <c r="A1101" t="s">
-        <v>3956</v>
+        <v>3955</v>
       </c>
       <c r="B1101" s="3" t="s">
         <v>243</v>
       </c>
       <c r="C1101" t="s">
+        <v>3956</v>
+      </c>
+      <c r="D1101" s="5" t="s">
         <v>3957</v>
-      </c>
-      <c r="D1101" s="5" t="s">
-        <v>3958</v>
       </c>
       <c r="E1101" t="s">
         <v>598</v>
@@ -34514,16 +34649,16 @@
     </row>
     <row r="1102" spans="1:6">
       <c r="A1102" t="s">
-        <v>3959</v>
+        <v>3958</v>
       </c>
       <c r="B1102" s="3" t="s">
         <v>114</v>
       </c>
       <c r="C1102" t="s">
+        <v>3959</v>
+      </c>
+      <c r="D1102" s="5" t="s">
         <v>3960</v>
-      </c>
-      <c r="D1102" s="5" t="s">
-        <v>3961</v>
       </c>
       <c r="E1102" t="s">
         <v>598</v>
@@ -34534,16 +34669,16 @@
     </row>
     <row r="1103" spans="1:6">
       <c r="A1103" t="s">
-        <v>3962</v>
+        <v>3961</v>
       </c>
       <c r="B1103" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C1103" t="s">
+        <v>3962</v>
+      </c>
+      <c r="D1103" s="5" t="s">
         <v>3963</v>
-      </c>
-      <c r="D1103" s="5" t="s">
-        <v>3964</v>
       </c>
       <c r="E1103" t="s">
         <v>598</v>
@@ -34554,16 +34689,16 @@
     </row>
     <row r="1104" spans="1:6">
       <c r="A1104" t="s">
-        <v>3965</v>
+        <v>3964</v>
       </c>
       <c r="B1104" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C1104" t="s">
+        <v>3965</v>
+      </c>
+      <c r="D1104" s="5" t="s">
         <v>3966</v>
-      </c>
-      <c r="D1104" s="5" t="s">
-        <v>3967</v>
       </c>
       <c r="E1104" t="s">
         <v>598</v>
@@ -34574,16 +34709,16 @@
     </row>
     <row r="1105" spans="1:6">
       <c r="A1105" t="s">
-        <v>3968</v>
+        <v>3967</v>
       </c>
       <c r="B1105" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C1105" t="s">
-        <v>3969</v>
+        <v>3968</v>
       </c>
       <c r="D1105" t="s">
-        <v>3970</v>
+        <v>4029</v>
       </c>
       <c r="E1105" t="s">
         <v>564</v>
@@ -34594,16 +34729,16 @@
     </row>
     <row r="1106" spans="1:6">
       <c r="A1106" t="s">
-        <v>3971</v>
+        <v>3969</v>
       </c>
       <c r="B1106" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C1106" t="s">
-        <v>4003</v>
+        <v>4001</v>
       </c>
       <c r="D1106" t="s">
-        <v>3987</v>
+        <v>3985</v>
       </c>
       <c r="E1106" t="s">
         <v>734</v>
@@ -34614,16 +34749,16 @@
     </row>
     <row r="1107" spans="1:6">
       <c r="A1107" t="s">
-        <v>3972</v>
+        <v>3970</v>
       </c>
       <c r="B1107" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C1107" t="s">
-        <v>4004</v>
+        <v>4002</v>
       </c>
       <c r="D1107" t="s">
-        <v>3988</v>
+        <v>3986</v>
       </c>
       <c r="E1107" t="s">
         <v>734</v>
@@ -34634,16 +34769,16 @@
     </row>
     <row r="1108" spans="1:6">
       <c r="A1108" t="s">
-        <v>3973</v>
+        <v>3971</v>
       </c>
       <c r="B1108" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C1108" t="s">
-        <v>4005</v>
+        <v>4003</v>
       </c>
       <c r="D1108" t="s">
-        <v>3989</v>
+        <v>3987</v>
       </c>
       <c r="E1108" t="s">
         <v>734</v>
@@ -34654,16 +34789,16 @@
     </row>
     <row r="1109" spans="1:6">
       <c r="A1109" t="s">
-        <v>3974</v>
+        <v>3972</v>
       </c>
       <c r="B1109" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C1109" t="s">
-        <v>4006</v>
+        <v>4004</v>
       </c>
       <c r="D1109" t="s">
-        <v>3990</v>
+        <v>3988</v>
       </c>
       <c r="E1109" t="s">
         <v>734</v>
@@ -34674,16 +34809,16 @@
     </row>
     <row r="1110" spans="1:6">
       <c r="A1110" t="s">
-        <v>3975</v>
+        <v>3973</v>
       </c>
       <c r="B1110" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C1110" t="s">
-        <v>4007</v>
+        <v>4005</v>
       </c>
       <c r="D1110" t="s">
-        <v>3991</v>
+        <v>3989</v>
       </c>
       <c r="E1110" t="s">
         <v>734</v>
@@ -34694,16 +34829,16 @@
     </row>
     <row r="1111" spans="1:6">
       <c r="A1111" t="s">
-        <v>3976</v>
+        <v>3974</v>
       </c>
       <c r="B1111" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C1111" t="s">
-        <v>4008</v>
+        <v>4006</v>
       </c>
       <c r="D1111" t="s">
-        <v>3992</v>
+        <v>3990</v>
       </c>
       <c r="E1111" t="s">
         <v>734</v>
@@ -34714,16 +34849,16 @@
     </row>
     <row r="1112" spans="1:6">
       <c r="A1112" t="s">
-        <v>3977</v>
+        <v>3975</v>
       </c>
       <c r="B1112" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C1112" t="s">
-        <v>4009</v>
+        <v>4007</v>
       </c>
       <c r="D1112" t="s">
-        <v>3993</v>
+        <v>3991</v>
       </c>
       <c r="E1112" t="s">
         <v>734</v>
@@ -34734,16 +34869,16 @@
     </row>
     <row r="1113" spans="1:6">
       <c r="A1113" t="s">
-        <v>3978</v>
+        <v>3976</v>
       </c>
       <c r="B1113" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C1113" t="s">
-        <v>4010</v>
+        <v>4008</v>
       </c>
       <c r="D1113" t="s">
-        <v>3994</v>
+        <v>3992</v>
       </c>
       <c r="E1113" t="s">
         <v>734</v>
@@ -34754,16 +34889,16 @@
     </row>
     <row r="1114" spans="1:6">
       <c r="A1114" t="s">
-        <v>3979</v>
+        <v>3977</v>
       </c>
       <c r="B1114" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C1114" t="s">
-        <v>4011</v>
+        <v>4009</v>
       </c>
       <c r="D1114" t="s">
-        <v>3995</v>
+        <v>3993</v>
       </c>
       <c r="E1114" t="s">
         <v>734</v>
@@ -34774,16 +34909,16 @@
     </row>
     <row r="1115" spans="1:6">
       <c r="A1115" t="s">
-        <v>3980</v>
+        <v>3978</v>
       </c>
       <c r="B1115" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C1115" t="s">
-        <v>4012</v>
+        <v>4010</v>
       </c>
       <c r="D1115" t="s">
-        <v>3996</v>
+        <v>3994</v>
       </c>
       <c r="E1115" t="s">
         <v>734</v>
@@ -34794,16 +34929,16 @@
     </row>
     <row r="1116" spans="1:6">
       <c r="A1116" t="s">
-        <v>3981</v>
+        <v>3979</v>
       </c>
       <c r="B1116" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C1116" t="s">
-        <v>4013</v>
+        <v>4011</v>
       </c>
       <c r="D1116" t="s">
-        <v>3997</v>
+        <v>3995</v>
       </c>
       <c r="E1116" t="s">
         <v>734</v>
@@ -34814,16 +34949,16 @@
     </row>
     <row r="1117" spans="1:6">
       <c r="A1117" t="s">
-        <v>3982</v>
+        <v>3980</v>
       </c>
       <c r="B1117" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C1117" t="s">
-        <v>4014</v>
+        <v>4012</v>
       </c>
       <c r="D1117" t="s">
-        <v>3998</v>
+        <v>3996</v>
       </c>
       <c r="E1117" t="s">
         <v>734</v>
@@ -34834,16 +34969,16 @@
     </row>
     <row r="1118" spans="1:6">
       <c r="A1118" t="s">
-        <v>3983</v>
+        <v>3981</v>
       </c>
       <c r="B1118" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C1118" t="s">
-        <v>4015</v>
+        <v>4013</v>
       </c>
       <c r="D1118" t="s">
-        <v>3999</v>
+        <v>3997</v>
       </c>
       <c r="E1118" t="s">
         <v>734</v>
@@ -34854,16 +34989,16 @@
     </row>
     <row r="1119" spans="1:6">
       <c r="A1119" t="s">
-        <v>3984</v>
+        <v>3982</v>
       </c>
       <c r="B1119" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C1119" t="s">
-        <v>4016</v>
+        <v>4014</v>
       </c>
       <c r="D1119" t="s">
-        <v>4000</v>
+        <v>3998</v>
       </c>
       <c r="E1119" t="s">
         <v>734</v>
@@ -34874,16 +35009,16 @@
     </row>
     <row r="1120" spans="1:6">
       <c r="A1120" t="s">
-        <v>3985</v>
+        <v>3983</v>
       </c>
       <c r="B1120" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C1120" t="s">
-        <v>4017</v>
+        <v>4015</v>
       </c>
       <c r="D1120" t="s">
-        <v>4001</v>
+        <v>3999</v>
       </c>
       <c r="E1120" t="s">
         <v>734</v>
@@ -34894,21 +35029,321 @@
     </row>
     <row r="1121" spans="1:6">
       <c r="A1121" t="s">
-        <v>3986</v>
+        <v>3984</v>
       </c>
       <c r="B1121" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C1121" t="s">
-        <v>4018</v>
+        <v>4016</v>
       </c>
       <c r="D1121" t="s">
-        <v>4002</v>
+        <v>4000</v>
       </c>
       <c r="E1121" t="s">
         <v>734</v>
       </c>
       <c r="F1121" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:6">
+      <c r="A1122" t="s">
+        <v>4017</v>
+      </c>
+      <c r="B1122" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1122" s="5" t="s">
+        <v>4019</v>
+      </c>
+      <c r="D1122" t="s">
+        <v>4018</v>
+      </c>
+      <c r="E1122" t="s">
+        <v>750</v>
+      </c>
+      <c r="F1122" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:6">
+      <c r="A1123" t="s">
+        <v>4022</v>
+      </c>
+      <c r="B1123" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C1123" t="s">
+        <v>4020</v>
+      </c>
+      <c r="D1123" s="5" t="s">
+        <v>4021</v>
+      </c>
+      <c r="E1123" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1123" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:6">
+      <c r="A1124" t="s">
+        <v>4025</v>
+      </c>
+      <c r="B1124" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1124" t="s">
+        <v>4023</v>
+      </c>
+      <c r="D1124" s="5" t="s">
+        <v>4024</v>
+      </c>
+      <c r="E1124" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1124" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:6">
+      <c r="A1125" t="s">
+        <v>4026</v>
+      </c>
+      <c r="B1125" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1125" t="s">
+        <v>4027</v>
+      </c>
+      <c r="D1125" t="s">
+        <v>4028</v>
+      </c>
+      <c r="E1125" t="s">
+        <v>564</v>
+      </c>
+      <c r="F1125" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:6">
+      <c r="A1126" t="s">
+        <v>4031</v>
+      </c>
+      <c r="B1126" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1126" t="s">
+        <v>4033</v>
+      </c>
+      <c r="D1126" s="5" t="s">
+        <v>4032</v>
+      </c>
+      <c r="E1126" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1126" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:6">
+      <c r="A1127" t="s">
+        <v>4036</v>
+      </c>
+      <c r="B1127" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C1127" t="s">
+        <v>4035</v>
+      </c>
+      <c r="D1127" t="s">
+        <v>4034</v>
+      </c>
+      <c r="E1127" t="s">
+        <v>564</v>
+      </c>
+      <c r="F1127" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:6">
+      <c r="A1128" t="s">
+        <v>4039</v>
+      </c>
+      <c r="B1128" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1128" t="s">
+        <v>4037</v>
+      </c>
+      <c r="D1128" t="s">
+        <v>4038</v>
+      </c>
+      <c r="E1128" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1128" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:6">
+      <c r="A1129" t="s">
+        <v>4042</v>
+      </c>
+      <c r="B1129" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1129" t="s">
+        <v>4040</v>
+      </c>
+      <c r="D1129" t="s">
+        <v>4041</v>
+      </c>
+      <c r="E1129" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1129" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:6">
+      <c r="A1130" t="s">
+        <v>4043</v>
+      </c>
+      <c r="B1130" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C1130" t="s">
+        <v>4044</v>
+      </c>
+      <c r="D1130" t="s">
+        <v>4045</v>
+      </c>
+      <c r="E1130" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1130" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:6">
+      <c r="A1131" t="s">
+        <v>4046</v>
+      </c>
+      <c r="B1131" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1131" t="s">
+        <v>4047</v>
+      </c>
+      <c r="D1131" t="s">
+        <v>4048</v>
+      </c>
+      <c r="E1131" t="s">
+        <v>564</v>
+      </c>
+      <c r="F1131" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:6">
+      <c r="A1132" t="s">
+        <v>4049</v>
+      </c>
+      <c r="B1132" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1132" t="s">
+        <v>4050</v>
+      </c>
+      <c r="D1132" t="s">
+        <v>4051</v>
+      </c>
+      <c r="E1132" t="s">
+        <v>564</v>
+      </c>
+      <c r="F1132" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:6">
+      <c r="A1133" t="s">
+        <v>4052</v>
+      </c>
+      <c r="B1133" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C1133" t="s">
+        <v>4054</v>
+      </c>
+      <c r="D1133" t="s">
+        <v>4053</v>
+      </c>
+      <c r="E1133" t="s">
+        <v>564</v>
+      </c>
+      <c r="F1133" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:6">
+      <c r="A1134" t="s">
+        <v>4055</v>
+      </c>
+      <c r="B1134" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1134" t="s">
+        <v>4056</v>
+      </c>
+      <c r="D1134" t="s">
+        <v>4057</v>
+      </c>
+      <c r="E1134" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1134" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:6">
+      <c r="A1135" t="s">
+        <v>4058</v>
+      </c>
+      <c r="B1135" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1135" t="s">
+        <v>4059</v>
+      </c>
+      <c r="D1135" t="s">
+        <v>4060</v>
+      </c>
+      <c r="E1135" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1135" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:6">
+      <c r="A1136" t="s">
+        <v>4061</v>
+      </c>
+      <c r="B1136" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1136" t="s">
+        <v>4062</v>
+      </c>
+      <c r="D1136" t="s">
+        <v>4063</v>
+      </c>
+      <c r="E1136" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1136" t="s">
         <v>3928</v>
       </c>
     </row>
@@ -34916,16 +35351,16 @@
   <autoFilter ref="A1:F1094"/>
   <dataValidations count="5">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C740">
-      <formula1>COUNTIF($C$2:$C$19945,C740)=1</formula1>
+      <formula1>COUNTIF($C$2:$C$19943,C740)=1</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D740">
-      <formula1>COUNTIF($D$2:$D$19945,D740)=1</formula1>
+      <formula1>COUNTIF($D$2:$D$19943,D740)=1</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C791">
-      <formula1>COUNTIF($C$2:$C$19937,C1477)=1</formula1>
+      <formula1>COUNTIF($C$2:$C$19935,C1475)=1</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D791">
-      <formula1>COUNTIF($D$2:$D$19937,D1477)=1</formula1>
+      <formula1>COUNTIF($D$2:$D$19935,D1475)=1</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D969 C1095:D1048576 C1071:D1093 C985:D1015 C970:D983 C1:D606 C774:D774 C741:D771 C608:D739 C783:C790 D775:D790 C879:D968 C1018:D1065 C775:C781 C792:D877">
       <formula1>COUNTIF(C:C,C1)=1</formula1>
@@ -35211,9 +35646,14 @@
     <hyperlink ref="D1102" r:id="rId277"/>
     <hyperlink ref="D1103" r:id="rId278"/>
     <hyperlink ref="D1104" r:id="rId279"/>
+    <hyperlink ref="C63" r:id="rId280"/>
+    <hyperlink ref="C1122" r:id="rId281"/>
+    <hyperlink ref="D1123" r:id="rId282"/>
+    <hyperlink ref="D1124" r:id="rId283"/>
+    <hyperlink ref="D1126" r:id="rId284"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId280"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId285"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -35221,7 +35661,7 @@
           <x14:formula1>
             <xm:f>Topics!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B1095:B1048576 B194:B263 B265:B354 B356:B408 B458 B417:B453 B497:B1093 B2:B192</xm:sqref>
+          <xm:sqref>B194:B263 B265:B354 B356:B408 B458 B417:B453 B497:B1093 B2:B192 B1095:B1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
server: add more feeds in excel
</commit_message>
<xml_diff>
--- a/server/cmd/tools/createfeeds/feeds.xlsx
+++ b/server/cmd/tools/createfeeds/feeds.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7467" uniqueCount="4064">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7491" uniqueCount="4076">
   <si>
     <t>TopicCode</t>
   </si>
@@ -12222,6 +12222,42 @@
   </si>
   <si>
     <t>https://www.koozarch.com/magazine</t>
+  </si>
+  <si>
+    <t>r/F1Porn</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/F1Porn/</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/F1Porn.rss</t>
+  </si>
+  <si>
+    <t>https://rss.app/feeds/p5jdBcBvWRtxMsuE.xml</t>
+  </si>
+  <si>
+    <t>https://www.nba.com/news</t>
+  </si>
+  <si>
+    <t>NBA News</t>
+  </si>
+  <si>
+    <t>https://api.foxsports.com/v2/content/optimized-rss?partnerKey=MB0Wehpmuj2lUhuRhQaafhBjAJqaPU244mlTDK1i&amp;size=30&amp;tags=fs/nba</t>
+  </si>
+  <si>
+    <t>https://www.foxsports.com/nba</t>
+  </si>
+  <si>
+    <t>Fox Sports NBA</t>
+  </si>
+  <si>
+    <t>Dunkest NBA</t>
+  </si>
+  <si>
+    <t>https://www.dunkest.com/en/rss/news/nba</t>
+  </si>
+  <si>
+    <t>https://www.dunkest.com/it/nba</t>
   </si>
 </sst>
 </file>
@@ -12611,10 +12647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1136"/>
+  <dimension ref="A1:F1140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1120" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A1137" sqref="A1137"/>
+    <sheetView tabSelected="1" topLeftCell="A1128" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A1141" sqref="A1141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -35344,6 +35380,86 @@
         <v>598</v>
       </c>
       <c r="F1136" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:6">
+      <c r="A1137" t="s">
+        <v>4064</v>
+      </c>
+      <c r="B1137" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1137" s="5" t="s">
+        <v>4066</v>
+      </c>
+      <c r="D1137" t="s">
+        <v>4065</v>
+      </c>
+      <c r="E1137" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1137" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:6">
+      <c r="A1138" t="s">
+        <v>4069</v>
+      </c>
+      <c r="B1138" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C1138" t="s">
+        <v>4067</v>
+      </c>
+      <c r="D1138" t="s">
+        <v>4068</v>
+      </c>
+      <c r="E1138" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1138" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:6">
+      <c r="A1139" t="s">
+        <v>4072</v>
+      </c>
+      <c r="B1139" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C1139" t="s">
+        <v>4070</v>
+      </c>
+      <c r="D1139" t="s">
+        <v>4071</v>
+      </c>
+      <c r="E1139" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1139" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:6">
+      <c r="A1140" t="s">
+        <v>4073</v>
+      </c>
+      <c r="B1140" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C1140" t="s">
+        <v>4074</v>
+      </c>
+      <c r="D1140" t="s">
+        <v>4075</v>
+      </c>
+      <c r="E1140" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1140" t="s">
         <v>3928</v>
       </c>
     </row>
@@ -35651,9 +35767,10 @@
     <hyperlink ref="D1123" r:id="rId282"/>
     <hyperlink ref="D1124" r:id="rId283"/>
     <hyperlink ref="D1126" r:id="rId284"/>
+    <hyperlink ref="C1137" r:id="rId285"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId285"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId286"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>

<commit_message>
server: mark admin added feeds as verfied and add new feeds in excel
</commit_message>
<xml_diff>
--- a/server/cmd/tools/createfeeds/feeds.xlsx
+++ b/server/cmd/tools/createfeeds/feeds.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7556" uniqueCount="4109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7591" uniqueCount="4127">
   <si>
     <t>TopicCode</t>
   </si>
@@ -12357,6 +12357,60 @@
   </si>
   <si>
     <t>https://www.reddit.com/r/Physics/</t>
+  </si>
+  <si>
+    <t>r/Pune</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/pune.rss</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/pune/</t>
+  </si>
+  <si>
+    <t>Scaffold - Podcast</t>
+  </si>
+  <si>
+    <t>https://feeds.acast.com/public/shows/622e82ac18ddd00014e37a58</t>
+  </si>
+  <si>
+    <t>http://architecturefoundation.org.uk</t>
+  </si>
+  <si>
+    <t>The National Archives - Blog</t>
+  </si>
+  <si>
+    <t>https://blog.nationalarchives.gov.uk/feed/</t>
+  </si>
+  <si>
+    <t>https://blog.nationalarchives.gov.uk/</t>
+  </si>
+  <si>
+    <t>The National Archives - News</t>
+  </si>
+  <si>
+    <t>https://www.nationalarchives.gov.uk/category/news/feed/</t>
+  </si>
+  <si>
+    <t>https://www.nationalarchives.gov.uk/category/about-us/news/</t>
+  </si>
+  <si>
+    <t>Heritage Trust Network UK</t>
+  </si>
+  <si>
+    <t>http://heritagetrustnetwork.org.uk/</t>
+  </si>
+  <si>
+    <t>https://heritagetrustnetwork.org.uk/feed/</t>
+  </si>
+  <si>
+    <t>dezeen jobs</t>
+  </si>
+  <si>
+    <t>https://www.dezeenjobs.com/feed/</t>
+  </si>
+  <si>
+    <t>https://www.dezeenjobs.com/</t>
   </si>
 </sst>
 </file>
@@ -12746,10 +12800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1151"/>
+  <dimension ref="A1:F1157"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1137" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A1152" sqref="A1152"/>
+      <selection activeCell="A1158" sqref="A1158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -35776,6 +35830,123 @@
         <v>734</v>
       </c>
       <c r="F1151" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:6">
+      <c r="A1152" t="s">
+        <v>4109</v>
+      </c>
+      <c r="C1152" t="s">
+        <v>4110</v>
+      </c>
+      <c r="D1152" s="5" t="s">
+        <v>4111</v>
+      </c>
+      <c r="E1152" t="s">
+        <v>734</v>
+      </c>
+      <c r="F1152" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:6">
+      <c r="A1153" t="s">
+        <v>4112</v>
+      </c>
+      <c r="B1153" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1153" t="s">
+        <v>4113</v>
+      </c>
+      <c r="D1153" t="s">
+        <v>4114</v>
+      </c>
+      <c r="E1153" t="s">
+        <v>3700</v>
+      </c>
+      <c r="F1153" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:6">
+      <c r="A1154" t="s">
+        <v>4115</v>
+      </c>
+      <c r="B1154" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1154" t="s">
+        <v>4116</v>
+      </c>
+      <c r="D1154" t="s">
+        <v>4117</v>
+      </c>
+      <c r="E1154" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1154" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:6">
+      <c r="A1155" t="s">
+        <v>4118</v>
+      </c>
+      <c r="B1155" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1155" t="s">
+        <v>4119</v>
+      </c>
+      <c r="D1155" t="s">
+        <v>4120</v>
+      </c>
+      <c r="E1155" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1155" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:6">
+      <c r="A1156" t="s">
+        <v>4121</v>
+      </c>
+      <c r="B1156" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1156" t="s">
+        <v>4123</v>
+      </c>
+      <c r="D1156" t="s">
+        <v>4122</v>
+      </c>
+      <c r="E1156" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1156" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:6">
+      <c r="A1157" t="s">
+        <v>4124</v>
+      </c>
+      <c r="B1157" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1157" t="s">
+        <v>4125</v>
+      </c>
+      <c r="D1157" s="5" t="s">
+        <v>4126</v>
+      </c>
+      <c r="E1157" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1157" t="s">
         <v>3928</v>
       </c>
     </row>
@@ -36087,9 +36258,11 @@
     <hyperlink ref="C1141" r:id="rId286"/>
     <hyperlink ref="D1141" r:id="rId287"/>
     <hyperlink ref="D1151" r:id="rId288"/>
+    <hyperlink ref="D1152" r:id="rId289"/>
+    <hyperlink ref="D1157" r:id="rId290"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId289"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId291"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>

<commit_message>
server: add new topics and feeds
</commit_message>
<xml_diff>
--- a/server/cmd/tools/createfeeds/feeds.xlsx
+++ b/server/cmd/tools/createfeeds/feeds.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7591" uniqueCount="4127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7695" uniqueCount="4182">
   <si>
     <t>TopicCode</t>
   </si>
@@ -12411,6 +12411,171 @@
   </si>
   <si>
     <t>https://www.dezeenjobs.com/</t>
+  </si>
+  <si>
+    <t>Aeon Magazine</t>
+  </si>
+  <si>
+    <t>philosophy</t>
+  </si>
+  <si>
+    <t>Philosophy</t>
+  </si>
+  <si>
+    <t>https://smphr.aravindunnikrishnan.in/static/images/topics/sm/philosophy.jpg</t>
+  </si>
+  <si>
+    <t>https://smphr.aravindunnikrishnan.in/static/images/topics/sm/agriculture.jpg</t>
+  </si>
+  <si>
+    <t>philhistory</t>
+  </si>
+  <si>
+    <t>Philosophy x History</t>
+  </si>
+  <si>
+    <t>artphil</t>
+  </si>
+  <si>
+    <t>Philosophy x Art</t>
+  </si>
+  <si>
+    <t>https://aeon.co/feed.rss</t>
+  </si>
+  <si>
+    <t>https://aeon.co</t>
+  </si>
+  <si>
+    <t>Big Think</t>
+  </si>
+  <si>
+    <t>https://bigthink.com//feed/all</t>
+  </si>
+  <si>
+    <t>https://bigthink.com/</t>
+  </si>
+  <si>
+    <t>Reason and Meaning</t>
+  </si>
+  <si>
+    <t>https://reasonandmeaning.com/feed/</t>
+  </si>
+  <si>
+    <t>https://reasonandmeaning.com/</t>
+  </si>
+  <si>
+    <t>Aesthetics for Birds</t>
+  </si>
+  <si>
+    <t>https://aestheticsforbirds.com/feed/</t>
+  </si>
+  <si>
+    <t>https://aestheticsforbirds.com/</t>
+  </si>
+  <si>
+    <t>The Indian Philosophy Blog</t>
+  </si>
+  <si>
+    <t>https://indianphilosophyblog.org/feed/</t>
+  </si>
+  <si>
+    <t>https://indianphilosophyblog.org</t>
+  </si>
+  <si>
+    <t>Daily Philosophy</t>
+  </si>
+  <si>
+    <t>https://daily-philosophy.com/index.xml</t>
+  </si>
+  <si>
+    <t>https://daily-philosophy.com/</t>
+  </si>
+  <si>
+    <t>https://www.evphil.com/blog/feed</t>
+  </si>
+  <si>
+    <t>https://www.evphil.com/blog</t>
+  </si>
+  <si>
+    <t>Evolutionary Philosophy Blog</t>
+  </si>
+  <si>
+    <t>Extinct Blog | The Philosophy of Palaeontology</t>
+  </si>
+  <si>
+    <t>https://www.extinctblog.org/extinct?format=rss</t>
+  </si>
+  <si>
+    <t>Journal of the History of Ideas Blog</t>
+  </si>
+  <si>
+    <t>https://www.jhiblog.org/</t>
+  </si>
+  <si>
+    <t>https://www.jhiblog.org/feed/</t>
+  </si>
+  <si>
+    <t>The Infinite Staircase</t>
+  </si>
+  <si>
+    <t>https://infinitestaircasebymoore.com/feed/</t>
+  </si>
+  <si>
+    <t>https://infinitestaircasebymoore.com/blog/</t>
+  </si>
+  <si>
+    <t>The Dawdler's Philosophy</t>
+  </si>
+  <si>
+    <t>https://www.dawdlersphilosophy.com/feed/</t>
+  </si>
+  <si>
+    <t>https://www.dawdlersphilosophy.com/category/blog/</t>
+  </si>
+  <si>
+    <t>A Philosopher's Blog</t>
+  </si>
+  <si>
+    <t>https://aphilosopher.drmcl.com/feed/</t>
+  </si>
+  <si>
+    <t>https://aphilosopher.drmcl.com/</t>
+  </si>
+  <si>
+    <t>Blog of the American Philosophical Association</t>
+  </si>
+  <si>
+    <t>https://blog.apaonline.org/feed/</t>
+  </si>
+  <si>
+    <t>https://blog.apaonline.org/</t>
+  </si>
+  <si>
+    <t>The Brains Blog</t>
+  </si>
+  <si>
+    <t>https://philosophyofbrains.com/</t>
+  </si>
+  <si>
+    <t>https://philosophyofbrains.com/feed</t>
+  </si>
+  <si>
+    <t>Arts and Letters Daily</t>
+  </si>
+  <si>
+    <t>https://www.aldaily.com/feed/</t>
+  </si>
+  <si>
+    <t>https://www.aldaily.com/</t>
+  </si>
+  <si>
+    <t>Daily Nous</t>
+  </si>
+  <si>
+    <t>https://dailynous.com/feed/</t>
+  </si>
+  <si>
+    <t>https://dailynous.com/</t>
   </si>
 </sst>
 </file>
@@ -12526,8 +12691,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C299" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:C299"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C302" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:C302"/>
   <tableColumns count="3">
     <tableColumn id="1" name="TopicCode"/>
     <tableColumn id="2" name="TopicName"/>
@@ -12800,10 +12965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1157"/>
+  <dimension ref="A1:F1173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1137" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A1158" sqref="A1158"/>
+    <sheetView tabSelected="1" topLeftCell="A1158" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A1174" sqref="A1174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -35947,6 +36112,326 @@
         <v>598</v>
       </c>
       <c r="F1157" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:6">
+      <c r="A1158" t="s">
+        <v>4127</v>
+      </c>
+      <c r="B1158" s="3" t="s">
+        <v>4128</v>
+      </c>
+      <c r="C1158" t="s">
+        <v>4136</v>
+      </c>
+      <c r="D1158" t="s">
+        <v>4137</v>
+      </c>
+      <c r="E1158" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1158" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:6">
+      <c r="A1159" t="s">
+        <v>4138</v>
+      </c>
+      <c r="B1159" s="3" t="s">
+        <v>4128</v>
+      </c>
+      <c r="C1159" t="s">
+        <v>4139</v>
+      </c>
+      <c r="D1159" t="s">
+        <v>4140</v>
+      </c>
+      <c r="E1159" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1159" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:6">
+      <c r="A1160" t="s">
+        <v>4141</v>
+      </c>
+      <c r="B1160" s="3" t="s">
+        <v>4128</v>
+      </c>
+      <c r="C1160" t="s">
+        <v>4142</v>
+      </c>
+      <c r="D1160" t="s">
+        <v>4143</v>
+      </c>
+      <c r="E1160" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1160" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:6">
+      <c r="A1161" t="s">
+        <v>4144</v>
+      </c>
+      <c r="B1161" s="3" t="s">
+        <v>4134</v>
+      </c>
+      <c r="C1161" t="s">
+        <v>4145</v>
+      </c>
+      <c r="D1161" t="s">
+        <v>4146</v>
+      </c>
+      <c r="E1161" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1161" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:6">
+      <c r="A1162" t="s">
+        <v>4147</v>
+      </c>
+      <c r="B1162" s="3" t="s">
+        <v>4128</v>
+      </c>
+      <c r="C1162" t="s">
+        <v>4148</v>
+      </c>
+      <c r="D1162" s="5" t="s">
+        <v>4149</v>
+      </c>
+      <c r="E1162" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1162" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:6">
+      <c r="A1163" t="s">
+        <v>4150</v>
+      </c>
+      <c r="B1163" s="3" t="s">
+        <v>4128</v>
+      </c>
+      <c r="C1163" t="s">
+        <v>4151</v>
+      </c>
+      <c r="D1163" t="s">
+        <v>4152</v>
+      </c>
+      <c r="E1163" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1163" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:6">
+      <c r="A1164" t="s">
+        <v>4155</v>
+      </c>
+      <c r="B1164" s="3" t="s">
+        <v>4128</v>
+      </c>
+      <c r="C1164" t="s">
+        <v>4153</v>
+      </c>
+      <c r="D1164" t="s">
+        <v>4154</v>
+      </c>
+      <c r="E1164" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1164" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:6">
+      <c r="A1165" t="s">
+        <v>4156</v>
+      </c>
+      <c r="B1165" s="3" t="s">
+        <v>4128</v>
+      </c>
+      <c r="C1165" t="s">
+        <v>4157</v>
+      </c>
+      <c r="D1165" t="s">
+        <v>4154</v>
+      </c>
+      <c r="E1165" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1165" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:6">
+      <c r="A1166" t="s">
+        <v>4158</v>
+      </c>
+      <c r="B1166" s="3" t="s">
+        <v>4132</v>
+      </c>
+      <c r="C1166" t="s">
+        <v>4160</v>
+      </c>
+      <c r="D1166" t="s">
+        <v>4159</v>
+      </c>
+      <c r="E1166" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1166" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:6">
+      <c r="A1167" t="s">
+        <v>4161</v>
+      </c>
+      <c r="B1167" s="3" t="s">
+        <v>4128</v>
+      </c>
+      <c r="C1167" t="s">
+        <v>4162</v>
+      </c>
+      <c r="D1167" t="s">
+        <v>4163</v>
+      </c>
+      <c r="E1167" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1167" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:6">
+      <c r="A1168" t="s">
+        <v>4164</v>
+      </c>
+      <c r="B1168" s="3" t="s">
+        <v>4128</v>
+      </c>
+      <c r="C1168" t="s">
+        <v>4165</v>
+      </c>
+      <c r="D1168" t="s">
+        <v>4166</v>
+      </c>
+      <c r="E1168" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1168" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:6">
+      <c r="A1169" t="s">
+        <v>4167</v>
+      </c>
+      <c r="B1169" s="3" t="s">
+        <v>4128</v>
+      </c>
+      <c r="C1169" t="s">
+        <v>4168</v>
+      </c>
+      <c r="D1169" t="s">
+        <v>4169</v>
+      </c>
+      <c r="E1169" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1169" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:6">
+      <c r="A1170" t="s">
+        <v>4170</v>
+      </c>
+      <c r="B1170" s="3" t="s">
+        <v>4128</v>
+      </c>
+      <c r="C1170" t="s">
+        <v>4171</v>
+      </c>
+      <c r="D1170" t="s">
+        <v>4172</v>
+      </c>
+      <c r="E1170" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1170" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:6">
+      <c r="A1171" t="s">
+        <v>4173</v>
+      </c>
+      <c r="B1171" s="3" t="s">
+        <v>4128</v>
+      </c>
+      <c r="C1171" t="s">
+        <v>4175</v>
+      </c>
+      <c r="D1171" t="s">
+        <v>4174</v>
+      </c>
+      <c r="E1171" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1171" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:6">
+      <c r="A1172" t="s">
+        <v>4176</v>
+      </c>
+      <c r="B1172" s="3" t="s">
+        <v>4134</v>
+      </c>
+      <c r="C1172" t="s">
+        <v>4177</v>
+      </c>
+      <c r="D1172" t="s">
+        <v>4178</v>
+      </c>
+      <c r="E1172" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1172" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:6">
+      <c r="A1173" t="s">
+        <v>4179</v>
+      </c>
+      <c r="B1173" s="3" t="s">
+        <v>4128</v>
+      </c>
+      <c r="C1173" t="s">
+        <v>4180</v>
+      </c>
+      <c r="D1173" t="s">
+        <v>4181</v>
+      </c>
+      <c r="E1173" t="s">
+        <v>598</v>
+      </c>
+      <c r="F1173" t="s">
         <v>3928</v>
       </c>
     </row>
@@ -36260,17 +36745,60 @@
     <hyperlink ref="D1151" r:id="rId288"/>
     <hyperlink ref="D1152" r:id="rId289"/>
     <hyperlink ref="D1157" r:id="rId290"/>
+    <hyperlink ref="D1162" r:id="rId291"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId291"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Topics!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B194:B263 B265:B354 B356:B408 B458 B417:B453 B497:B1093 B2:B192 B1095:B1048576</xm:sqref>
+          <xm:sqref>B194:B263</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Topics!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>B265:B354</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Topics!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>B356:B408</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Topics!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>B458</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Topics!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>B417:B453</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Topics!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>B497:B1093</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Topics!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B192</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Topics!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1095:B1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -36280,10 +36808,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C299"/>
+  <dimension ref="A1:C302"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C46"/>
+    <sheetView topLeftCell="A289" workbookViewId="0">
+      <selection activeCell="A303" sqref="A303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -36333,6 +36861,9 @@
       <c r="B4" t="s">
         <v>269</v>
       </c>
+      <c r="C4" s="5" t="s">
+        <v>4131</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
@@ -36699,2131 +37230,2161 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>4128</v>
       </c>
       <c r="B38" t="s">
-        <v>303</v>
+        <v>4129</v>
       </c>
       <c r="C38" t="s">
-        <v>3918</v>
+        <v>4130</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B39" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C39" t="s">
-        <v>3919</v>
+        <v>3918</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>265</v>
+        <v>80</v>
       </c>
       <c r="B40" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C40" t="s">
-        <v>3920</v>
+        <v>3919</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>265</v>
       </c>
       <c r="B41" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C41" t="s">
-        <v>3921</v>
+        <v>3920</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B42" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C42" t="s">
-        <v>3922</v>
+        <v>3921</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>266</v>
+        <v>82</v>
       </c>
       <c r="B43" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C43" t="s">
-        <v>3923</v>
+        <v>3922</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>83</v>
+        <v>266</v>
       </c>
       <c r="B44" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C44" t="s">
-        <v>3924</v>
+        <v>3923</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B45" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C45" t="s">
-        <v>3925</v>
+        <v>3924</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B46" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C46" t="s">
-        <v>3926</v>
+        <v>3925</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="B47" t="s">
-        <v>312</v>
+        <v>311</v>
+      </c>
+      <c r="C47" t="s">
+        <v>3926</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B48" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B49" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B50" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>706</v>
+        <v>28</v>
       </c>
       <c r="B51" t="s">
-        <v>707</v>
+        <v>315</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>29</v>
+        <v>706</v>
       </c>
       <c r="B52" t="s">
-        <v>316</v>
+        <v>707</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B53" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B54" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B55" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B57" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B58" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B59" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B60" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B61" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B62" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B63" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B64" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B65" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B66" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B67" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B68" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B69" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B70" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B71" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B72" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B73" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B74" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B75" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B76" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B77" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B78" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B79" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B80" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B81" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B82" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B83" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B84" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B85" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B86" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B87" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B88" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B89" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B90" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B91" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B92" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B93" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B94" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B95" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B96" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B97" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B98" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B99" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B100" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B101" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B102" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B103" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B104" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>1757</v>
+        <v>90</v>
       </c>
       <c r="B105" t="s">
-        <v>1758</v>
+        <v>368</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>91</v>
+        <v>1757</v>
       </c>
       <c r="B106" t="s">
-        <v>369</v>
+        <v>1758</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B107" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B108" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B109" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B110" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B111" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B112" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B113" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B114" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B115" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B116" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B117" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B118" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B119" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B120" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B121" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B122" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B123" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B124" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B125" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B126" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B127" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B128" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B129" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B130" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B131" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B132" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B133" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B134" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B135" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B136" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B137" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B138" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B139" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B140" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B141" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B142" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B143" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B144" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B145" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B146" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B147" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B148" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B149" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B150" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B151" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B152" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B153" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B154" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B155" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B156" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B157" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B158" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B159" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B160" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B161" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B162" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B163" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B164" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B165" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B166" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B167" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B168" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B169" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B170" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B171" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B172" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B173" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B174" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B175" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B176" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B177" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B178" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B179" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B180" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B181" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B182" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B183" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B184" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B185" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B186" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B187" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B188" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B189" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B190" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B191" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B192" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B193" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B194" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B195" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B196" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B197" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B198" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B199" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B200" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B201" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B202" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B203" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B204" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B205" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B206" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B207" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B208" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B209" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B210" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B211" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B212" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B213" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B214" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="215" spans="1:2">
       <c r="A215" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B215" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B216" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="217" spans="1:2">
       <c r="A217" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B217" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="218" spans="1:2">
       <c r="A218" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B218" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="219" spans="1:2">
       <c r="A219" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B219" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B220" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="221" spans="1:2">
       <c r="A221" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B221" t="s">
-        <v>291</v>
+        <v>483</v>
       </c>
     </row>
     <row r="222" spans="1:2">
       <c r="A222" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B222" t="s">
-        <v>484</v>
+        <v>291</v>
       </c>
     </row>
     <row r="223" spans="1:2">
       <c r="A223" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B223" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="224" spans="1:2">
       <c r="A224" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B224" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B225" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B226" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B227" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B228" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B229" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B230" t="s">
-        <v>309</v>
+        <v>491</v>
       </c>
     </row>
     <row r="231" spans="1:2">
       <c r="A231" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B231" t="s">
-        <v>492</v>
+        <v>309</v>
       </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B232" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="233" spans="1:2">
       <c r="A233" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B233" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B234" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="235" spans="1:2">
       <c r="A235" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B235" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="236" spans="1:2">
       <c r="A236" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B236" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="237" spans="1:2">
       <c r="A237" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B237" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="238" spans="1:2">
       <c r="A238" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B238" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="239" spans="1:2">
       <c r="A239" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B239" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="240" spans="1:2">
       <c r="A240" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B240" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="241" spans="1:2">
       <c r="A241" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B241" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="242" spans="1:2">
       <c r="A242" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B242" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="243" spans="1:2">
       <c r="A243" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B243" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="244" spans="1:2">
       <c r="A244" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B244" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="245" spans="1:2">
       <c r="A245" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B245" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="246" spans="1:2">
       <c r="A246" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B246" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="247" spans="1:2">
       <c r="A247" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B247" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="248" spans="1:2">
       <c r="A248" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B248" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="249" spans="1:2">
       <c r="A249" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B249" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="250" spans="1:2">
       <c r="A250" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B250" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="251" spans="1:2">
       <c r="A251" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B251" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B252" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="253" spans="1:2">
       <c r="A253" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B253" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="254" spans="1:2">
       <c r="A254" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B254" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="255" spans="1:2">
       <c r="A255" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B255" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="256" spans="1:2">
       <c r="A256" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B256" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="257" spans="1:2">
       <c r="A257" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B257" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="258" spans="1:2">
       <c r="A258" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B258" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="259" spans="1:2">
       <c r="A259" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B259" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="260" spans="1:2">
       <c r="A260" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B260" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="261" spans="1:2">
       <c r="A261" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B261" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="262" spans="1:2">
       <c r="A262" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B262" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="263" spans="1:2">
       <c r="A263" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B263" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="264" spans="1:2">
       <c r="A264" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B264" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="265" spans="1:2">
       <c r="A265" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B265" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="266" spans="1:2">
       <c r="A266" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B266" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="267" spans="1:2">
       <c r="A267" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B267" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="268" spans="1:2">
       <c r="A268" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B268" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="269" spans="1:2">
       <c r="A269" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B269" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="270" spans="1:2">
       <c r="A270" t="s">
-        <v>536</v>
+        <v>254</v>
       </c>
       <c r="B270" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
     </row>
     <row r="271" spans="1:2">
       <c r="A271" t="s">
-        <v>593</v>
+        <v>536</v>
       </c>
       <c r="B271" t="s">
-        <v>594</v>
+        <v>537</v>
       </c>
     </row>
     <row r="272" spans="1:2">
       <c r="A272" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B272" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="273" spans="1:2">
       <c r="A273" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="B273" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
     </row>
     <row r="274" spans="1:2">
       <c r="A274" t="s">
+        <v>601</v>
+      </c>
+      <c r="B274" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2">
+      <c r="A275" t="s">
         <v>668</v>
       </c>
-      <c r="B274" t="s">
+      <c r="B275" t="s">
         <v>671</v>
       </c>
     </row>
-    <row r="275" spans="1:2">
-      <c r="A275" s="4" t="s">
+    <row r="276" spans="1:2">
+      <c r="A276" s="4" t="s">
         <v>637</v>
       </c>
-      <c r="B275" t="s">
+      <c r="B276" t="s">
         <v>672</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2">
-      <c r="A276" t="s">
-        <v>657</v>
-      </c>
-      <c r="B276" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="277" spans="1:2">
       <c r="A277" t="s">
-        <v>676</v>
+        <v>657</v>
       </c>
       <c r="B277" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
     </row>
     <row r="278" spans="1:2">
       <c r="A278" t="s">
-        <v>708</v>
+        <v>676</v>
       </c>
       <c r="B278" t="s">
-        <v>709</v>
+        <v>677</v>
       </c>
     </row>
     <row r="279" spans="1:2">
       <c r="A279" t="s">
-        <v>924</v>
+        <v>708</v>
       </c>
       <c r="B279" t="s">
-        <v>925</v>
+        <v>709</v>
       </c>
     </row>
     <row r="280" spans="1:2">
       <c r="A280" t="s">
-        <v>1095</v>
+        <v>924</v>
       </c>
       <c r="B280" t="s">
-        <v>1096</v>
+        <v>925</v>
       </c>
     </row>
     <row r="281" spans="1:2">
       <c r="A281" t="s">
-        <v>1417</v>
+        <v>1095</v>
       </c>
       <c r="B281" t="s">
-        <v>1418</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="282" spans="1:2">
       <c r="A282" t="s">
-        <v>1502</v>
+        <v>1417</v>
       </c>
       <c r="B282" t="s">
-        <v>1503</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="283" spans="1:2">
       <c r="A283" t="s">
-        <v>1548</v>
+        <v>1502</v>
       </c>
       <c r="B283" t="s">
-        <v>1549</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="284" spans="1:2">
       <c r="A284" t="s">
-        <v>1910</v>
+        <v>1548</v>
       </c>
       <c r="B284" t="s">
-        <v>1911</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="285" spans="1:2">
       <c r="A285" t="s">
-        <v>1912</v>
+        <v>1910</v>
       </c>
       <c r="B285" t="s">
-        <v>1913</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="286" spans="1:2">
       <c r="A286" t="s">
-        <v>2018</v>
+        <v>1912</v>
       </c>
       <c r="B286" t="s">
-        <v>2019</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="287" spans="1:2">
       <c r="A287" t="s">
-        <v>2325</v>
+        <v>2018</v>
       </c>
       <c r="B287" t="s">
-        <v>2326</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="288" spans="1:2">
       <c r="A288" t="s">
-        <v>2382</v>
+        <v>2325</v>
       </c>
       <c r="B288" t="s">
-        <v>2383</v>
+        <v>2326</v>
       </c>
     </row>
     <row r="289" spans="1:2">
       <c r="A289" t="s">
-        <v>2558</v>
+        <v>2382</v>
       </c>
       <c r="B289" t="s">
-        <v>2559</v>
+        <v>2383</v>
       </c>
     </row>
     <row r="290" spans="1:2">
       <c r="A290" t="s">
-        <v>2650</v>
+        <v>2558</v>
       </c>
       <c r="B290" t="s">
-        <v>2651</v>
+        <v>2559</v>
       </c>
     </row>
     <row r="291" spans="1:2">
       <c r="A291" t="s">
-        <v>2830</v>
+        <v>2650</v>
       </c>
       <c r="B291" t="s">
-        <v>2831</v>
+        <v>2651</v>
       </c>
     </row>
     <row r="292" spans="1:2">
       <c r="A292" t="s">
-        <v>3040</v>
+        <v>2830</v>
       </c>
       <c r="B292" t="s">
-        <v>3041</v>
+        <v>2831</v>
       </c>
     </row>
     <row r="293" spans="1:2">
       <c r="A293" t="s">
-        <v>3042</v>
+        <v>3040</v>
       </c>
       <c r="B293" t="s">
-        <v>3043</v>
+        <v>3041</v>
       </c>
     </row>
     <row r="294" spans="1:2">
       <c r="A294" t="s">
-        <v>3044</v>
+        <v>3042</v>
       </c>
       <c r="B294" t="s">
-        <v>3045</v>
+        <v>3043</v>
       </c>
     </row>
     <row r="295" spans="1:2">
       <c r="A295" t="s">
-        <v>3461</v>
+        <v>3044</v>
       </c>
       <c r="B295" t="s">
-        <v>3462</v>
+        <v>3045</v>
       </c>
     </row>
     <row r="296" spans="1:2">
       <c r="A296" t="s">
-        <v>3548</v>
+        <v>3461</v>
       </c>
       <c r="B296" t="s">
-        <v>3549</v>
+        <v>3462</v>
       </c>
     </row>
     <row r="297" spans="1:2">
       <c r="A297" t="s">
-        <v>3691</v>
+        <v>3548</v>
       </c>
       <c r="B297" t="s">
-        <v>3692</v>
+        <v>3549</v>
       </c>
     </row>
     <row r="298" spans="1:2">
       <c r="A298" t="s">
-        <v>3836</v>
+        <v>3691</v>
       </c>
       <c r="B298" t="s">
-        <v>3837</v>
+        <v>3692</v>
       </c>
     </row>
     <row r="299" spans="1:2">
       <c r="A299" t="s">
+        <v>3836</v>
+      </c>
+      <c r="B299" t="s">
+        <v>3837</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2">
+      <c r="A300" t="s">
         <v>3838</v>
       </c>
-      <c r="B299" t="s">
+      <c r="B300" t="s">
         <v>3839</v>
       </c>
     </row>
+    <row r="301" spans="1:2">
+      <c r="A301" t="s">
+        <v>4132</v>
+      </c>
+      <c r="B301" t="s">
+        <v>4133</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2">
+      <c r="A302" t="s">
+        <v>4134</v>
+      </c>
+      <c r="B302" t="s">
+        <v>4135</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
server: minor update to big think feed
</commit_message>
<xml_diff>
--- a/server/cmd/tools/createfeeds/feeds.xlsx
+++ b/server/cmd/tools/createfeeds/feeds.xlsx
@@ -12449,9 +12449,6 @@
     <t>Big Think</t>
   </si>
   <si>
-    <t>https://bigthink.com//feed/all</t>
-  </si>
-  <si>
     <t>https://bigthink.com/</t>
   </si>
   <si>
@@ -12576,6 +12573,9 @@
   </si>
   <si>
     <t>https://dailynous.com/</t>
+  </si>
+  <si>
+    <t>https://bigthink.com/feed/</t>
   </si>
 </sst>
 </file>
@@ -12968,7 +12968,7 @@
   <dimension ref="A1:F1173"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1158" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A1174" sqref="A1174"/>
+      <selection activeCell="C1160" sqref="C1160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -36142,11 +36142,11 @@
       <c r="B1159" s="3" t="s">
         <v>4128</v>
       </c>
-      <c r="C1159" t="s">
+      <c r="C1159" s="5" t="s">
+        <v>4181</v>
+      </c>
+      <c r="D1159" t="s">
         <v>4139</v>
-      </c>
-      <c r="D1159" t="s">
-        <v>4140</v>
       </c>
       <c r="E1159" t="s">
         <v>598</v>
@@ -36157,16 +36157,16 @@
     </row>
     <row r="1160" spans="1:6">
       <c r="A1160" t="s">
-        <v>4141</v>
+        <v>4140</v>
       </c>
       <c r="B1160" s="3" t="s">
         <v>4128</v>
       </c>
       <c r="C1160" t="s">
+        <v>4141</v>
+      </c>
+      <c r="D1160" t="s">
         <v>4142</v>
-      </c>
-      <c r="D1160" t="s">
-        <v>4143</v>
       </c>
       <c r="E1160" t="s">
         <v>598</v>
@@ -36177,16 +36177,16 @@
     </row>
     <row r="1161" spans="1:6">
       <c r="A1161" t="s">
-        <v>4144</v>
+        <v>4143</v>
       </c>
       <c r="B1161" s="3" t="s">
         <v>4134</v>
       </c>
       <c r="C1161" t="s">
+        <v>4144</v>
+      </c>
+      <c r="D1161" t="s">
         <v>4145</v>
-      </c>
-      <c r="D1161" t="s">
-        <v>4146</v>
       </c>
       <c r="E1161" t="s">
         <v>598</v>
@@ -36197,16 +36197,16 @@
     </row>
     <row r="1162" spans="1:6">
       <c r="A1162" t="s">
-        <v>4147</v>
+        <v>4146</v>
       </c>
       <c r="B1162" s="3" t="s">
         <v>4128</v>
       </c>
       <c r="C1162" t="s">
+        <v>4147</v>
+      </c>
+      <c r="D1162" s="5" t="s">
         <v>4148</v>
-      </c>
-      <c r="D1162" s="5" t="s">
-        <v>4149</v>
       </c>
       <c r="E1162" t="s">
         <v>598</v>
@@ -36217,16 +36217,16 @@
     </row>
     <row r="1163" spans="1:6">
       <c r="A1163" t="s">
-        <v>4150</v>
+        <v>4149</v>
       </c>
       <c r="B1163" s="3" t="s">
         <v>4128</v>
       </c>
       <c r="C1163" t="s">
+        <v>4150</v>
+      </c>
+      <c r="D1163" t="s">
         <v>4151</v>
-      </c>
-      <c r="D1163" t="s">
-        <v>4152</v>
       </c>
       <c r="E1163" t="s">
         <v>598</v>
@@ -36237,16 +36237,16 @@
     </row>
     <row r="1164" spans="1:6">
       <c r="A1164" t="s">
-        <v>4155</v>
+        <v>4154</v>
       </c>
       <c r="B1164" s="3" t="s">
         <v>4128</v>
       </c>
       <c r="C1164" t="s">
+        <v>4152</v>
+      </c>
+      <c r="D1164" t="s">
         <v>4153</v>
-      </c>
-      <c r="D1164" t="s">
-        <v>4154</v>
       </c>
       <c r="E1164" t="s">
         <v>598</v>
@@ -36257,16 +36257,16 @@
     </row>
     <row r="1165" spans="1:6">
       <c r="A1165" t="s">
-        <v>4156</v>
+        <v>4155</v>
       </c>
       <c r="B1165" s="3" t="s">
         <v>4128</v>
       </c>
       <c r="C1165" t="s">
-        <v>4157</v>
+        <v>4156</v>
       </c>
       <c r="D1165" t="s">
-        <v>4154</v>
+        <v>4153</v>
       </c>
       <c r="E1165" t="s">
         <v>598</v>
@@ -36277,16 +36277,16 @@
     </row>
     <row r="1166" spans="1:6">
       <c r="A1166" t="s">
-        <v>4158</v>
+        <v>4157</v>
       </c>
       <c r="B1166" s="3" t="s">
         <v>4132</v>
       </c>
       <c r="C1166" t="s">
-        <v>4160</v>
+        <v>4159</v>
       </c>
       <c r="D1166" t="s">
-        <v>4159</v>
+        <v>4158</v>
       </c>
       <c r="E1166" t="s">
         <v>598</v>
@@ -36297,16 +36297,16 @@
     </row>
     <row r="1167" spans="1:6">
       <c r="A1167" t="s">
-        <v>4161</v>
+        <v>4160</v>
       </c>
       <c r="B1167" s="3" t="s">
         <v>4128</v>
       </c>
       <c r="C1167" t="s">
+        <v>4161</v>
+      </c>
+      <c r="D1167" t="s">
         <v>4162</v>
-      </c>
-      <c r="D1167" t="s">
-        <v>4163</v>
       </c>
       <c r="E1167" t="s">
         <v>598</v>
@@ -36317,16 +36317,16 @@
     </row>
     <row r="1168" spans="1:6">
       <c r="A1168" t="s">
-        <v>4164</v>
+        <v>4163</v>
       </c>
       <c r="B1168" s="3" t="s">
         <v>4128</v>
       </c>
       <c r="C1168" t="s">
+        <v>4164</v>
+      </c>
+      <c r="D1168" t="s">
         <v>4165</v>
-      </c>
-      <c r="D1168" t="s">
-        <v>4166</v>
       </c>
       <c r="E1168" t="s">
         <v>598</v>
@@ -36337,16 +36337,16 @@
     </row>
     <row r="1169" spans="1:6">
       <c r="A1169" t="s">
-        <v>4167</v>
+        <v>4166</v>
       </c>
       <c r="B1169" s="3" t="s">
         <v>4128</v>
       </c>
       <c r="C1169" t="s">
+        <v>4167</v>
+      </c>
+      <c r="D1169" t="s">
         <v>4168</v>
-      </c>
-      <c r="D1169" t="s">
-        <v>4169</v>
       </c>
       <c r="E1169" t="s">
         <v>598</v>
@@ -36357,16 +36357,16 @@
     </row>
     <row r="1170" spans="1:6">
       <c r="A1170" t="s">
-        <v>4170</v>
+        <v>4169</v>
       </c>
       <c r="B1170" s="3" t="s">
         <v>4128</v>
       </c>
       <c r="C1170" t="s">
+        <v>4170</v>
+      </c>
+      <c r="D1170" t="s">
         <v>4171</v>
-      </c>
-      <c r="D1170" t="s">
-        <v>4172</v>
       </c>
       <c r="E1170" t="s">
         <v>598</v>
@@ -36377,16 +36377,16 @@
     </row>
     <row r="1171" spans="1:6">
       <c r="A1171" t="s">
-        <v>4173</v>
+        <v>4172</v>
       </c>
       <c r="B1171" s="3" t="s">
         <v>4128</v>
       </c>
       <c r="C1171" t="s">
-        <v>4175</v>
+        <v>4174</v>
       </c>
       <c r="D1171" t="s">
-        <v>4174</v>
+        <v>4173</v>
       </c>
       <c r="E1171" t="s">
         <v>598</v>
@@ -36397,16 +36397,16 @@
     </row>
     <row r="1172" spans="1:6">
       <c r="A1172" t="s">
-        <v>4176</v>
+        <v>4175</v>
       </c>
       <c r="B1172" s="3" t="s">
         <v>4134</v>
       </c>
       <c r="C1172" t="s">
+        <v>4176</v>
+      </c>
+      <c r="D1172" t="s">
         <v>4177</v>
-      </c>
-      <c r="D1172" t="s">
-        <v>4178</v>
       </c>
       <c r="E1172" t="s">
         <v>598</v>
@@ -36417,16 +36417,16 @@
     </row>
     <row r="1173" spans="1:6">
       <c r="A1173" t="s">
-        <v>4179</v>
+        <v>4178</v>
       </c>
       <c r="B1173" s="3" t="s">
         <v>4128</v>
       </c>
       <c r="C1173" t="s">
+        <v>4179</v>
+      </c>
+      <c r="D1173" t="s">
         <v>4180</v>
-      </c>
-      <c r="D1173" t="s">
-        <v>4181</v>
       </c>
       <c r="E1173" t="s">
         <v>598</v>
@@ -36746,9 +36746,10 @@
     <hyperlink ref="D1152" r:id="rId289"/>
     <hyperlink ref="D1157" r:id="rId290"/>
     <hyperlink ref="D1162" r:id="rId291"/>
+    <hyperlink ref="C1159" r:id="rId292"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId292"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId293"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">

</xml_diff>